<commit_message>
update to get bioproject accession for ncbit
</commit_message>
<xml_diff>
--- a/runs/osu867/ncbi_mapping/ncbi_submission_data/osu867_SRA_metadata.xlsx
+++ b/runs/osu867/ncbi_mapping/ncbi_submission_data/osu867_SRA_metadata.xlsx
@@ -1329,12 +1329,12 @@
     <row r="2">
       <c r="A2" s="18" t="inlineStr">
         <is>
-          <t>E24.NC.DY2012</t>
+          <t>E24.NC.DY20-12</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>E24.NC.DY2012_Parada16S_osu867</t>
+          <t>E24.NC.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D2" s="11" t="inlineStr">
@@ -1391,12 +1391,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>E41.NC.DY2012</t>
+          <t>E41.NC.DY20-12</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>E41.NC.DY2012_Parada16S_osu867</t>
+          <t>E41.NC.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D3" s="11" t="inlineStr">
@@ -1453,12 +1453,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>E56.NC.DY2012</t>
+          <t>E56.NC.DY20-12</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>E56.NC.DY2012_Parada16S_osu867</t>
+          <t>E56.NC.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D4" s="11" t="inlineStr">
@@ -1515,12 +1515,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>E73.NC.DY2012</t>
+          <t>E73.NC.DY20-12</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>E73.NC.DY2012_Parada16S_osu867</t>
+          <t>E73.NC.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D5" s="11" t="inlineStr">
@@ -1701,12 +1701,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>E25.2B.DY2012</t>
+          <t>E25.2B.DY20-12</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>E25.2B.DY2012_Parada16S_osu867</t>
+          <t>E25.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D8" s="11" t="inlineStr">
@@ -1763,12 +1763,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>E26.1B.DY2012</t>
+          <t>E26.1B.DY20-12</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>E26.1B.DY2012_Parada16S_osu867</t>
+          <t>E26.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D9" s="11" t="inlineStr">
@@ -1825,12 +1825,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>E26.2B.DY2012</t>
+          <t>E26.2B.DY20-12</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>E26.2B.DY2012_Parada16S_osu867</t>
+          <t>E26.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D10" s="11" t="inlineStr">
@@ -1887,12 +1887,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>E27.1B.DY2012</t>
+          <t>E27.1B.DY20-12</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>E27.1B.DY2012_Parada16S_osu867</t>
+          <t>E27.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D11" s="11" t="inlineStr">
@@ -1949,12 +1949,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>E27.2B.DY2012</t>
+          <t>E27.2B.DY20-12</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>E27.2B.DY2012_Parada16S_osu867</t>
+          <t>E27.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D12" s="11" t="inlineStr">
@@ -2011,12 +2011,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>E28.1B.DY2012</t>
+          <t>E28.1B.DY20-12</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>E28.1B.DY2012_Parada16S_osu867</t>
+          <t>E28.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D13" s="11" t="inlineStr">
@@ -2073,12 +2073,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>E28.2B.DY2012</t>
+          <t>E28.2B.DY20-12</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>E28.2B.DY2012_Parada16S_osu867</t>
+          <t>E28.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D14" s="11" t="inlineStr">
@@ -2135,12 +2135,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>E29.1B.DY2012</t>
+          <t>E29.1B.DY20-12</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>E29.1B.DY2012_Parada16S_osu867</t>
+          <t>E29.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D15" s="11" t="inlineStr">
@@ -2197,12 +2197,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>E29.2B.DY2012</t>
+          <t>E29.2B.DY20-12</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>E29.2B.DY2012_Parada16S_osu867</t>
+          <t>E29.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D16" s="11" t="inlineStr">
@@ -2259,12 +2259,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>E30.1B.DY2012</t>
+          <t>E30.1B.DY20-12</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>E30.1B.DY2012_Parada16S_osu867</t>
+          <t>E30.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D17" s="11" t="inlineStr">
@@ -2321,12 +2321,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>E30.2B.DY2012</t>
+          <t>E30.2B.DY20-12</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>E30.2B.DY2012_Parada16S_osu867</t>
+          <t>E30.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D18" s="11" t="inlineStr">
@@ -2383,12 +2383,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>E31.1B.DY2012</t>
+          <t>E31.1B.DY20-12</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>E31.1B.DY2012_Parada16S_osu867</t>
+          <t>E31.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D19" s="11" t="inlineStr">
@@ -2445,12 +2445,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>E31.2B.DY2012</t>
+          <t>E31.2B.DY20-12</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>E31.2B.DY2012_Parada16S_osu867</t>
+          <t>E31.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D20" s="11" t="inlineStr">
@@ -2507,12 +2507,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>E32.1B.DY2012</t>
+          <t>E32.1B.DY20-12</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>E32.1B.DY2012_Parada16S_osu867</t>
+          <t>E32.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D21" s="11" t="inlineStr">
@@ -2569,12 +2569,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>E32.2B.DY2012</t>
+          <t>E32.2B.DY20-12</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>E32.2B.DY2012_Parada16S_osu867</t>
+          <t>E32.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D22" s="11" t="inlineStr">
@@ -2631,12 +2631,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>E33.1B.DY2012</t>
+          <t>E33.1B.DY20-12</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>E33.1B.DY2012_Parada16S_osu867</t>
+          <t>E33.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D23" s="11" t="inlineStr">
@@ -2693,12 +2693,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>E33.2B.DY2012</t>
+          <t>E33.2B.DY20-12</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>E33.2B.DY2012_Parada16S_osu867</t>
+          <t>E33.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D24" s="11" t="inlineStr">
@@ -2755,12 +2755,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>E34.1B.DY2012</t>
+          <t>E34.1B.DY20-12</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>E34.1B.DY2012_Parada16S_osu867</t>
+          <t>E34.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D25" s="11" t="inlineStr">
@@ -2817,12 +2817,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>E34.2B.DY2012</t>
+          <t>E34.2B.DY20-12</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>E34.2B.DY2012_Parada16S_osu867</t>
+          <t>E34.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D26" s="11" t="inlineStr">
@@ -2879,12 +2879,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>E35.1B.DY2012</t>
+          <t>E35.1B.DY20-12</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>E35.1B.DY2012_Parada16S_osu867</t>
+          <t>E35.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D27" s="11" t="inlineStr">
@@ -2941,12 +2941,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>E35.2B.DY2012</t>
+          <t>E35.2B.DY20-12</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>E35.2B.DY2012_Parada16S_osu867</t>
+          <t>E35.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D28" s="11" t="inlineStr">
@@ -3003,12 +3003,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>E36.1B.DY2012</t>
+          <t>E36.1B.DY20-12</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>E36.1B.DY2012_Parada16S_osu867</t>
+          <t>E36.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D29" s="11" t="inlineStr">
@@ -3065,12 +3065,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>E36.2B.DY2012</t>
+          <t>E36.2B.DY20-12</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>E36.2B.DY2012_Parada16S_osu867</t>
+          <t>E36.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D30" s="11" t="inlineStr">
@@ -3127,12 +3127,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>E37.1B.DY2012</t>
+          <t>E37.1B.DY20-12</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>E37.1B.DY2012_Parada16S_osu867</t>
+          <t>E37.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D31" s="11" t="inlineStr">
@@ -3189,12 +3189,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>E37.2B.DY2012</t>
+          <t>E37.2B.DY20-12</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>E37.2B.DY2012_Parada16S_osu867</t>
+          <t>E37.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D32" s="11" t="inlineStr">
@@ -3251,12 +3251,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>E38.1B.DY2012</t>
+          <t>E38.1B.DY20-12</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>E38.1B.DY2012_Parada16S_osu867</t>
+          <t>E38.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D33" s="11" t="inlineStr">
@@ -3313,12 +3313,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>E38.2B.DY2012</t>
+          <t>E38.2B.DY20-12</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>E38.2B.DY2012_Parada16S_osu867</t>
+          <t>E38.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D34" s="11" t="inlineStr">
@@ -3375,12 +3375,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>E39.1B.DY2012</t>
+          <t>E39.1B.DY20-12</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>E39.1B.DY2012_Parada16S_osu867</t>
+          <t>E39.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D35" s="11" t="inlineStr">
@@ -3437,12 +3437,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>E39.2B.DY2012</t>
+          <t>E39.2B.DY20-12</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>E39.2B.DY2012_Parada16S_osu867</t>
+          <t>E39.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D36" s="11" t="inlineStr">
@@ -3499,12 +3499,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>E40.1B.DY2012</t>
+          <t>E40.1B.DY20-12</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>E40.1B.DY2012_Parada16S_osu867</t>
+          <t>E40.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D37" s="11" t="inlineStr">
@@ -3561,12 +3561,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>E40.2B.DY2012</t>
+          <t>E40.2B.DY20-12</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>E40.2B.DY2012_Parada16S_osu867</t>
+          <t>E40.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D38" s="11" t="inlineStr">
@@ -3623,12 +3623,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>E42.1B.DY2012</t>
+          <t>E42.1B.DY20-12</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>E42.1B.DY2012_Parada16S_osu867</t>
+          <t>E42.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D39" s="11" t="inlineStr">
@@ -3685,12 +3685,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>E42.2B.DY2012</t>
+          <t>E42.2B.DY20-12</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>E42.2B.DY2012_Parada16S_osu867</t>
+          <t>E42.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D40" s="11" t="inlineStr">
@@ -3747,12 +3747,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>E43.1B.DY2012</t>
+          <t>E43.1B.DY20-12</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>E43.1B.DY2012_Parada16S_osu867</t>
+          <t>E43.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D41" s="11" t="inlineStr">
@@ -3809,12 +3809,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>E43.2B.DY2012</t>
+          <t>E43.2B.DY20-12</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>E43.2B.DY2012_Parada16S_osu867</t>
+          <t>E43.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D42" s="11" t="inlineStr">
@@ -3871,12 +3871,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>E44.DY2012</t>
+          <t>E44.DY20-12</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>E44.DY2012_Parada16S_osu867</t>
+          <t>E44.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D43" s="11" t="inlineStr">
@@ -3933,12 +3933,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>E45.1B.DY2012</t>
+          <t>E45.1B.DY20-12</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>E45.1B.DY2012_Parada16S_osu867</t>
+          <t>E45.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D44" s="11" t="inlineStr">
@@ -3995,12 +3995,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>E45.2B.DY2012</t>
+          <t>E45.2B.DY20-12</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>E45.2B.DY2012_Parada16S_osu867</t>
+          <t>E45.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D45" s="11" t="inlineStr">
@@ -4057,12 +4057,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>E46.1B.DY2012</t>
+          <t>E46.1B.DY20-12</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>E46.1B.DY2012_Parada16S_osu867</t>
+          <t>E46.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D46" s="11" t="inlineStr">
@@ -4119,12 +4119,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>E46.2B.DY2012</t>
+          <t>E46.2B.DY20-12</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>E46.2B.DY2012_Parada16S_osu867</t>
+          <t>E46.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D47" s="11" t="inlineStr">
@@ -4181,12 +4181,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>E47.1B.DY2012</t>
+          <t>E47.1B.DY20-12</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>E47.1B.DY2012_Parada16S_osu867</t>
+          <t>E47.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D48" s="11" t="inlineStr">
@@ -4243,12 +4243,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>E47.2B.DY2012</t>
+          <t>E47.2B.DY20-12</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>E47.2B.DY2012_Parada16S_osu867</t>
+          <t>E47.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D49" s="11" t="inlineStr">
@@ -4305,12 +4305,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>E48.1B.DY2012</t>
+          <t>E48.1B.DY20-12</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>E48.1B.DY2012_Parada16S_osu867</t>
+          <t>E48.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D50" s="11" t="inlineStr">
@@ -4367,12 +4367,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>E48.2B.DY2012</t>
+          <t>E48.2B.DY20-12</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>E48.2B.DY2012_Parada16S_osu867</t>
+          <t>E48.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D51" s="11" t="inlineStr">
@@ -4429,12 +4429,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>E49.1B.DY2012</t>
+          <t>E49.1B.DY20-12</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>E49.1B.DY2012_Parada16S_osu867</t>
+          <t>E49.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D52" s="11" t="inlineStr">
@@ -4491,12 +4491,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>E49.2B.DY2012</t>
+          <t>E49.2B.DY20-12</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>E49.2B.DY2012_Parada16S_osu867</t>
+          <t>E49.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D53" s="11" t="inlineStr">
@@ -4553,12 +4553,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>E50.1B.DY2012</t>
+          <t>E50.1B.DY20-12</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>E50.1B.DY2012_Parada16S_osu867</t>
+          <t>E50.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D54" s="11" t="inlineStr">
@@ -4615,12 +4615,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>E50.2B.DY2012</t>
+          <t>E50.2B.DY20-12</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>E50.2B.DY2012_Parada16S_osu867</t>
+          <t>E50.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D55" s="11" t="inlineStr">
@@ -4677,12 +4677,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>E51.1B.DY2012</t>
+          <t>E51.1B.DY20-12</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>E51.1B.DY2012_Parada16S_osu867</t>
+          <t>E51.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D56" s="11" t="inlineStr">
@@ -4739,12 +4739,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>E51.2B.DY2012</t>
+          <t>E51.2B.DY20-12</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>E51.2B.DY2012_Parada16S_osu867</t>
+          <t>E51.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D57" s="11" t="inlineStr">
@@ -4801,12 +4801,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>E52.1B.DY2012</t>
+          <t>E52.1B.DY20-12</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>E52.1B.DY2012_Parada16S_osu867</t>
+          <t>E52.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D58" s="11" t="inlineStr">
@@ -4863,12 +4863,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>E52.2B.DY2012</t>
+          <t>E52.2B.DY20-12</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>E52.2B.DY2012_Parada16S_osu867</t>
+          <t>E52.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D59" s="11" t="inlineStr">
@@ -4925,12 +4925,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>E53.1B.DY2012</t>
+          <t>E53.1B.DY20-12</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>E53.1B.DY2012_Parada16S_osu867</t>
+          <t>E53.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D60" s="11" t="inlineStr">
@@ -4987,12 +4987,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>E53.2B.DY2012</t>
+          <t>E53.2B.DY20-12</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>E53.2B.DY2012_Parada16S_osu867</t>
+          <t>E53.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D61" s="11" t="inlineStr">
@@ -5049,12 +5049,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>E54.1B.DY2012</t>
+          <t>E54.1B.DY20-12</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>E54.1B.DY2012_Parada16S_osu867</t>
+          <t>E54.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D62" s="11" t="inlineStr">
@@ -5111,12 +5111,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>E54.2B.DY2012</t>
+          <t>E54.2B.DY20-12</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>E54.2B.DY2012_Parada16S_osu867</t>
+          <t>E54.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D63" s="11" t="inlineStr">
@@ -5173,12 +5173,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>E55.1B.DY2012</t>
+          <t>E55.1B.DY20-12</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>E55.1B.DY2012_Parada16S_osu867</t>
+          <t>E55.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D64" s="11" t="inlineStr">
@@ -5235,12 +5235,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>E55.2B.DY2012</t>
+          <t>E55.2B.DY20-12</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>E55.2B.DY2012_Parada16S_osu867</t>
+          <t>E55.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D65" s="11" t="inlineStr">
@@ -5297,12 +5297,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>E57.1B.DY2012</t>
+          <t>E57.1B.DY20-12</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>E57.1B.DY2012_Parada16S_osu867</t>
+          <t>E57.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D66" s="11" t="inlineStr">
@@ -5359,12 +5359,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>E57.2B.DY2012</t>
+          <t>E57.2B.DY20-12</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>E57.2B.DY2012_Parada16S_osu867</t>
+          <t>E57.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D67" s="11" t="inlineStr">
@@ -5421,12 +5421,12 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>E58.1B.DY2012</t>
+          <t>E58.1B.DY20-12</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>E58.1B.DY2012_Parada16S_osu867</t>
+          <t>E58.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D68" s="11" t="inlineStr">
@@ -5483,12 +5483,12 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>E58.2B.DY2012</t>
+          <t>E58.2B.DY20-12</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>E58.2B.DY2012_Parada16S_osu867</t>
+          <t>E58.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D69" s="11" t="inlineStr">
@@ -5545,12 +5545,12 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>E59.1B.DY2012</t>
+          <t>E59.1B.DY20-12</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>E59.1B.DY2012_Parada16S_osu867</t>
+          <t>E59.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D70" s="11" t="inlineStr">
@@ -5607,12 +5607,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>E59.2B.DY2012</t>
+          <t>E59.2B.DY20-12</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>E59.2B.DY2012_Parada16S_osu867</t>
+          <t>E59.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D71" s="11" t="inlineStr">
@@ -5669,12 +5669,12 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>E60.1B.DY2012</t>
+          <t>E60.1B.DY20-12</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>E60.1B.DY2012_Parada16S_osu867</t>
+          <t>E60.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D72" s="11" t="inlineStr">
@@ -5731,12 +5731,12 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>E60.2B.DY2012</t>
+          <t>E60.2B.DY20-12</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>E60.2B.DY2012_Parada16S_osu867</t>
+          <t>E60.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D73" s="11" t="inlineStr">
@@ -5793,12 +5793,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>E61.1B.DY2012</t>
+          <t>E61.1B.DY20-12</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>E61.1B.DY2012_Parada16S_osu867</t>
+          <t>E61.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D74" s="11" t="inlineStr">
@@ -5855,12 +5855,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>E61.2B.DY2012</t>
+          <t>E61.2B.DY20-12</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>E61.2B.DY2012_Parada16S_osu867</t>
+          <t>E61.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D75" s="11" t="inlineStr">
@@ -5917,12 +5917,12 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>E62.1B.DY2012</t>
+          <t>E62.1B.DY20-12</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>E62.1B.DY2012_Parada16S_osu867</t>
+          <t>E62.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D76" s="11" t="inlineStr">
@@ -5979,12 +5979,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>E62.2B.DY2012</t>
+          <t>E62.2B.DY20-12</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>E62.2B.DY2012_Parada16S_osu867</t>
+          <t>E62.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D77" s="11" t="inlineStr">
@@ -6041,12 +6041,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>E63.1B.DY2012</t>
+          <t>E63.1B.DY20-12</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>E63.1B.DY2012_Parada16S_osu867</t>
+          <t>E63.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D78" s="11" t="inlineStr">
@@ -6103,12 +6103,12 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>E63.2B.DY2012</t>
+          <t>E63.2B.DY20-12</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>E63.2B.DY2012_Parada16S_osu867</t>
+          <t>E63.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D79" s="11" t="inlineStr">
@@ -6165,12 +6165,12 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>E64.1B.DY2012</t>
+          <t>E64.1B.DY20-12</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>E64.1B.DY2012_Parada16S_osu867</t>
+          <t>E64.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D80" s="11" t="inlineStr">
@@ -6227,12 +6227,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>E64.2B.DY2012</t>
+          <t>E64.2B.DY20-12</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>E64.2B.DY2012_Parada16S_osu867</t>
+          <t>E64.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D81" s="11" t="inlineStr">
@@ -6289,12 +6289,12 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>E65.1B.DY2012</t>
+          <t>E65.1B.DY20-12</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>E65.1B.DY2012_Parada16S_osu867</t>
+          <t>E65.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D82" s="11" t="inlineStr">
@@ -6351,12 +6351,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>E65.2B.DY2012</t>
+          <t>E65.2B.DY20-12</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>E65.2B.DY2012_Parada16S_osu867</t>
+          <t>E65.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D83" s="11" t="inlineStr">
@@ -6413,12 +6413,12 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>E66.1B.DY2012</t>
+          <t>E66.1B.DY20-12</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>E66.1B.DY2012_Parada16S_osu867</t>
+          <t>E66.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D84" s="11" t="inlineStr">
@@ -6475,12 +6475,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>E66.2B.DY2012</t>
+          <t>E66.2B.DY20-12</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>E66.2B.DY2012_Parada16S_osu867</t>
+          <t>E66.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D85" s="11" t="inlineStr">
@@ -6537,12 +6537,12 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>E67.1B.DY2012</t>
+          <t>E67.1B.DY20-12</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>E67.1B.DY2012_Parada16S_osu867</t>
+          <t>E67.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D86" s="11" t="inlineStr">
@@ -6599,12 +6599,12 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>E67.2B.DY2012</t>
+          <t>E67.2B.DY20-12</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>E67.2B.DY2012_Parada16S_osu867</t>
+          <t>E67.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D87" s="11" t="inlineStr">
@@ -6661,12 +6661,12 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>E68.1B.DY2012</t>
+          <t>E68.1B.DY20-12</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>E68.1B.DY2012_Parada16S_osu867</t>
+          <t>E68.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D88" s="11" t="inlineStr">
@@ -6723,12 +6723,12 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>E68.2B.DY2012</t>
+          <t>E68.2B.DY20-12</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>E68.2B.DY2012_Parada16S_osu867</t>
+          <t>E68.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D89" s="11" t="inlineStr">
@@ -6785,12 +6785,12 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>E69.1B.DY2012</t>
+          <t>E69.1B.DY20-12</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>E69.1B.DY2012_Parada16S_osu867</t>
+          <t>E69.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D90" s="11" t="inlineStr">
@@ -6847,12 +6847,12 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>E69.2B.DY2012</t>
+          <t>E69.2B.DY20-12</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>E69.2B.DY2012_Parada16S_osu867</t>
+          <t>E69.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D91" s="11" t="inlineStr">
@@ -6909,12 +6909,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>E70.1B.DY2012</t>
+          <t>E70.1B.DY20-12</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>E70.1B.DY2012_Parada16S_osu867</t>
+          <t>E70.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D92" s="11" t="inlineStr">
@@ -6971,12 +6971,12 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>E70.2B.DY2012</t>
+          <t>E70.2B.DY20-12</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>E70.2B.DY2012_Parada16S_osu867</t>
+          <t>E70.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D93" s="11" t="inlineStr">
@@ -7033,12 +7033,12 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>E71.1B.DY2012</t>
+          <t>E71.1B.DY20-12</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>E71.1B.DY2012_Parada16S_osu867</t>
+          <t>E71.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D94" s="11" t="inlineStr">
@@ -7095,12 +7095,12 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>E71.2B.DY2012</t>
+          <t>E71.2B.DY20-12</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>E71.2B.DY2012_Parada16S_osu867</t>
+          <t>E71.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D95" s="11" t="inlineStr">
@@ -7157,12 +7157,12 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>E72.1B.DY2012</t>
+          <t>E72.1B.DY20-12</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>E72.1B.DY2012_Parada16S_osu867</t>
+          <t>E72.1B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D96" s="11" t="inlineStr">
@@ -7219,12 +7219,12 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>E72.2B.DY2012</t>
+          <t>E72.2B.DY20-12</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>E72.2B.DY2012_Parada16S_osu867</t>
+          <t>E72.2B.DY20-12_Parada16S_osu867</t>
         </is>
       </c>
       <c r="D97" s="11" t="inlineStr">
@@ -7281,12 +7281,12 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>E24.NC.DY2012</t>
+          <t>E24.NC.DY20-12</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>E24.NC.DY2012_Machida18S_osu867</t>
+          <t>E24.NC.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D98" s="11" t="inlineStr">
@@ -7343,12 +7343,12 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>E41.NC.DY2012</t>
+          <t>E41.NC.DY20-12</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>E41.NC.DY2012_Machida18S_osu867</t>
+          <t>E41.NC.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D99" s="11" t="inlineStr">
@@ -7405,12 +7405,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>E56.NC.DY2012</t>
+          <t>E56.NC.DY20-12</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>E56.NC.DY2012_Machida18S_osu867</t>
+          <t>E56.NC.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D100" s="11" t="inlineStr">
@@ -7467,12 +7467,12 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>E73.NC.DY2012</t>
+          <t>E73.NC.DY20-12</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>E73.NC.DY2012_Machida18S_osu867</t>
+          <t>E73.NC.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D101" s="11" t="inlineStr">
@@ -7653,12 +7653,12 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>E25.2B.DY2012</t>
+          <t>E25.2B.DY20-12</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>E25.2B.DY2012_Machida18S_osu867</t>
+          <t>E25.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D104" s="11" t="inlineStr">
@@ -7715,12 +7715,12 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>E26.1B.DY2012</t>
+          <t>E26.1B.DY20-12</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>E26.1B.DY2012_Machida18S_osu867</t>
+          <t>E26.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D105" s="11" t="inlineStr">
@@ -7777,12 +7777,12 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>E26.2B.DY2012</t>
+          <t>E26.2B.DY20-12</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>E26.2B.DY2012_Machida18S_osu867</t>
+          <t>E26.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D106" s="11" t="inlineStr">
@@ -7839,12 +7839,12 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>E27.1B.DY2012</t>
+          <t>E27.1B.DY20-12</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>E27.1B.DY2012_Machida18S_osu867</t>
+          <t>E27.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D107" s="11" t="inlineStr">
@@ -7901,12 +7901,12 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>E27.2B.DY2012</t>
+          <t>E27.2B.DY20-12</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>E27.2B.DY2012_Machida18S_osu867</t>
+          <t>E27.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D108" s="11" t="inlineStr">
@@ -7963,12 +7963,12 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>E28.1B.DY2012</t>
+          <t>E28.1B.DY20-12</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>E28.1B.DY2012_Machida18S_osu867</t>
+          <t>E28.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D109" s="11" t="inlineStr">
@@ -8025,12 +8025,12 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>E28.2B.DY2012</t>
+          <t>E28.2B.DY20-12</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>E28.2B.DY2012_Machida18S_osu867</t>
+          <t>E28.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D110" s="11" t="inlineStr">
@@ -8087,12 +8087,12 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>E29.1B.DY2012</t>
+          <t>E29.1B.DY20-12</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>E29.1B.DY2012_Machida18S_osu867</t>
+          <t>E29.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D111" s="11" t="inlineStr">
@@ -8149,12 +8149,12 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>E29.2B.DY2012</t>
+          <t>E29.2B.DY20-12</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>E29.2B.DY2012_Machida18S_osu867</t>
+          <t>E29.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D112" s="11" t="inlineStr">
@@ -8211,12 +8211,12 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>E30.1B.DY2012</t>
+          <t>E30.1B.DY20-12</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>E30.1B.DY2012_Machida18S_osu867</t>
+          <t>E30.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D113" s="11" t="inlineStr">
@@ -8273,12 +8273,12 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>E30.2B.DY2012</t>
+          <t>E30.2B.DY20-12</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>E30.2B.DY2012_Machida18S_osu867</t>
+          <t>E30.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D114" s="11" t="inlineStr">
@@ -8335,12 +8335,12 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>E31.1B.DY2012</t>
+          <t>E31.1B.DY20-12</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>E31.1B.DY2012_Machida18S_osu867</t>
+          <t>E31.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D115" s="11" t="inlineStr">
@@ -8397,12 +8397,12 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>E31.2B.DY2012</t>
+          <t>E31.2B.DY20-12</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>E31.2B.DY2012_Machida18S_osu867</t>
+          <t>E31.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D116" s="11" t="inlineStr">
@@ -8459,12 +8459,12 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>E32.1B.DY2012</t>
+          <t>E32.1B.DY20-12</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>E32.1B.DY2012_Machida18S_osu867</t>
+          <t>E32.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D117" s="11" t="inlineStr">
@@ -8521,12 +8521,12 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>E32.2B.DY2012</t>
+          <t>E32.2B.DY20-12</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>E32.2B.DY2012_Machida18S_osu867</t>
+          <t>E32.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D118" s="11" t="inlineStr">
@@ -8583,12 +8583,12 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>E33.1B.DY2012</t>
+          <t>E33.1B.DY20-12</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>E33.1B.DY2012_Machida18S_osu867</t>
+          <t>E33.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D119" s="11" t="inlineStr">
@@ -8645,12 +8645,12 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>E33.2B.DY2012</t>
+          <t>E33.2B.DY20-12</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>E33.2B.DY2012_Machida18S_osu867</t>
+          <t>E33.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D120" s="11" t="inlineStr">
@@ -8707,12 +8707,12 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>E34.1B.DY2012</t>
+          <t>E34.1B.DY20-12</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>E34.1B.DY2012_Machida18S_osu867</t>
+          <t>E34.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D121" s="11" t="inlineStr">
@@ -8769,12 +8769,12 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>E34.2B.DY2012</t>
+          <t>E34.2B.DY20-12</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>E34.2B.DY2012_Machida18S_osu867</t>
+          <t>E34.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D122" s="11" t="inlineStr">
@@ -8831,12 +8831,12 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>E35.1B.DY2012</t>
+          <t>E35.1B.DY20-12</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>E35.1B.DY2012_Machida18S_osu867</t>
+          <t>E35.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D123" s="11" t="inlineStr">
@@ -8893,12 +8893,12 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>E35.2B.DY2012</t>
+          <t>E35.2B.DY20-12</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>E35.2B.DY2012_Machida18S_osu867</t>
+          <t>E35.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D124" s="11" t="inlineStr">
@@ -8955,12 +8955,12 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>E36.1B.DY2012</t>
+          <t>E36.1B.DY20-12</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>E36.1B.DY2012_Machida18S_osu867</t>
+          <t>E36.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D125" s="11" t="inlineStr">
@@ -9017,12 +9017,12 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>E36.2B.DY2012</t>
+          <t>E36.2B.DY20-12</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>E36.2B.DY2012_Machida18S_osu867</t>
+          <t>E36.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D126" s="11" t="inlineStr">
@@ -9079,12 +9079,12 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>E37.1B.DY2012</t>
+          <t>E37.1B.DY20-12</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>E37.1B.DY2012_Machida18S_osu867</t>
+          <t>E37.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D127" s="11" t="inlineStr">
@@ -9141,12 +9141,12 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>E37.2B.DY2012</t>
+          <t>E37.2B.DY20-12</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>E37.2B.DY2012_Machida18S_osu867</t>
+          <t>E37.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D128" s="11" t="inlineStr">
@@ -9203,12 +9203,12 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>E38.1B.DY2012</t>
+          <t>E38.1B.DY20-12</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>E38.1B.DY2012_Machida18S_osu867</t>
+          <t>E38.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D129" s="11" t="inlineStr">
@@ -9265,12 +9265,12 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>E38.2B.DY2012</t>
+          <t>E38.2B.DY20-12</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>E38.2B.DY2012_Machida18S_osu867</t>
+          <t>E38.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D130" s="11" t="inlineStr">
@@ -9327,12 +9327,12 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>E39.1B.DY2012</t>
+          <t>E39.1B.DY20-12</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>E39.1B.DY2012_Machida18S_osu867</t>
+          <t>E39.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D131" s="11" t="inlineStr">
@@ -9389,12 +9389,12 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>E39.2B.DY2012</t>
+          <t>E39.2B.DY20-12</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>E39.2B.DY2012_Machida18S_osu867</t>
+          <t>E39.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D132" s="11" t="inlineStr">
@@ -9451,12 +9451,12 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>E40.1B.DY2012</t>
+          <t>E40.1B.DY20-12</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>E40.1B.DY2012_Machida18S_osu867</t>
+          <t>E40.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D133" s="11" t="inlineStr">
@@ -9513,12 +9513,12 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>E40.2B.DY2012</t>
+          <t>E40.2B.DY20-12</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>E40.2B.DY2012_Machida18S_osu867</t>
+          <t>E40.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D134" s="11" t="inlineStr">
@@ -9575,12 +9575,12 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>E42.1B.DY2012</t>
+          <t>E42.1B.DY20-12</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>E42.1B.DY2012_Machida18S_osu867</t>
+          <t>E42.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D135" s="11" t="inlineStr">
@@ -9637,12 +9637,12 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>E42.2B.DY2012</t>
+          <t>E42.2B.DY20-12</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>E42.2B.DY2012_Machida18S_osu867</t>
+          <t>E42.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D136" s="11" t="inlineStr">
@@ -9699,12 +9699,12 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>E43.1B.DY2012</t>
+          <t>E43.1B.DY20-12</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>E43.1B.DY2012_Machida18S_osu867</t>
+          <t>E43.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D137" s="11" t="inlineStr">
@@ -9761,12 +9761,12 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>E43.2B.DY2012</t>
+          <t>E43.2B.DY20-12</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>E43.2B.DY2012_Machida18S_osu867</t>
+          <t>E43.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D138" s="11" t="inlineStr">
@@ -9823,12 +9823,12 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>E44.DY2012</t>
+          <t>E44.DY20-12</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>E44.DY2012_Machida18S_osu867</t>
+          <t>E44.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D139" s="11" t="inlineStr">
@@ -9885,12 +9885,12 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>E45.1B.DY2012</t>
+          <t>E45.1B.DY20-12</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>E45.1B.DY2012_Machida18S_osu867</t>
+          <t>E45.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D140" s="11" t="inlineStr">
@@ -9947,12 +9947,12 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>E45.2B.DY2012</t>
+          <t>E45.2B.DY20-12</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>E45.2B.DY2012_Machida18S_osu867</t>
+          <t>E45.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D141" s="11" t="inlineStr">
@@ -10009,12 +10009,12 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>E46.1B.DY2012</t>
+          <t>E46.1B.DY20-12</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>E46.1B.DY2012_Machida18S_osu867</t>
+          <t>E46.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D142" s="11" t="inlineStr">
@@ -10071,12 +10071,12 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>E46.2B.DY2012</t>
+          <t>E46.2B.DY20-12</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>E46.2B.DY2012_Machida18S_osu867</t>
+          <t>E46.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D143" s="11" t="inlineStr">
@@ -10133,12 +10133,12 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>E47.1B.DY2012</t>
+          <t>E47.1B.DY20-12</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>E47.1B.DY2012_Machida18S_osu867</t>
+          <t>E47.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D144" s="11" t="inlineStr">
@@ -10195,12 +10195,12 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>E47.2B.DY2012</t>
+          <t>E47.2B.DY20-12</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>E47.2B.DY2012_Machida18S_osu867</t>
+          <t>E47.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D145" s="11" t="inlineStr">
@@ -10257,12 +10257,12 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>E48.1B.DY2012</t>
+          <t>E48.1B.DY20-12</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>E48.1B.DY2012_Machida18S_osu867</t>
+          <t>E48.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D146" s="11" t="inlineStr">
@@ -10319,12 +10319,12 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>E48.2B.DY2012</t>
+          <t>E48.2B.DY20-12</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>E48.2B.DY2012_Machida18S_osu867</t>
+          <t>E48.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D147" s="11" t="inlineStr">
@@ -10381,12 +10381,12 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>E49.1B.DY2012</t>
+          <t>E49.1B.DY20-12</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>E49.1B.DY2012_Machida18S_osu867</t>
+          <t>E49.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D148" s="11" t="inlineStr">
@@ -10443,12 +10443,12 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>E49.2B.DY2012</t>
+          <t>E49.2B.DY20-12</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>E49.2B.DY2012_Machida18S_osu867</t>
+          <t>E49.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D149" s="11" t="inlineStr">
@@ -10505,12 +10505,12 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>E50.1B.DY2012</t>
+          <t>E50.1B.DY20-12</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>E50.1B.DY2012_Machida18S_osu867</t>
+          <t>E50.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D150" s="11" t="inlineStr">
@@ -10567,12 +10567,12 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>E50.2B.DY2012</t>
+          <t>E50.2B.DY20-12</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>E50.2B.DY2012_Machida18S_osu867</t>
+          <t>E50.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D151" s="11" t="inlineStr">
@@ -10629,12 +10629,12 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>E51.1B.DY2012</t>
+          <t>E51.1B.DY20-12</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>E51.1B.DY2012_Machida18S_osu867</t>
+          <t>E51.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D152" s="11" t="inlineStr">
@@ -10691,12 +10691,12 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>E51.2B.DY2012</t>
+          <t>E51.2B.DY20-12</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>E51.2B.DY2012_Machida18S_osu867</t>
+          <t>E51.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D153" s="11" t="inlineStr">
@@ -10753,12 +10753,12 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>E52.1B.DY2012</t>
+          <t>E52.1B.DY20-12</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>E52.1B.DY2012_Machida18S_osu867</t>
+          <t>E52.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D154" s="11" t="inlineStr">
@@ -10815,12 +10815,12 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>E52.2B.DY2012</t>
+          <t>E52.2B.DY20-12</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>E52.2B.DY2012_Machida18S_osu867</t>
+          <t>E52.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D155" s="11" t="inlineStr">
@@ -10877,12 +10877,12 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>E53.1B.DY2012</t>
+          <t>E53.1B.DY20-12</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>E53.1B.DY2012_Machida18S_osu867</t>
+          <t>E53.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D156" s="11" t="inlineStr">
@@ -10939,12 +10939,12 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>E53.2B.DY2012</t>
+          <t>E53.2B.DY20-12</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>E53.2B.DY2012_Machida18S_osu867</t>
+          <t>E53.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D157" s="11" t="inlineStr">
@@ -11001,12 +11001,12 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>E54.1B.DY2012</t>
+          <t>E54.1B.DY20-12</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>E54.1B.DY2012_Machida18S_osu867</t>
+          <t>E54.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D158" s="11" t="inlineStr">
@@ -11063,12 +11063,12 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>E54.2B.DY2012</t>
+          <t>E54.2B.DY20-12</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>E54.2B.DY2012_Machida18S_osu867</t>
+          <t>E54.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D159" s="11" t="inlineStr">
@@ -11125,12 +11125,12 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>E55.1B.DY2012</t>
+          <t>E55.1B.DY20-12</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>E55.1B.DY2012_Machida18S_osu867</t>
+          <t>E55.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D160" s="11" t="inlineStr">
@@ -11187,12 +11187,12 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>E55.2B.DY2012</t>
+          <t>E55.2B.DY20-12</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>E55.2B.DY2012_Machida18S_osu867</t>
+          <t>E55.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D161" s="11" t="inlineStr">
@@ -11249,12 +11249,12 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>E57.1B.DY2012</t>
+          <t>E57.1B.DY20-12</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>E57.1B.DY2012_Machida18S_osu867</t>
+          <t>E57.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D162" s="11" t="inlineStr">
@@ -11311,12 +11311,12 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>E57.2B.DY2012</t>
+          <t>E57.2B.DY20-12</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>E57.2B.DY2012_Machida18S_osu867</t>
+          <t>E57.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D163" s="11" t="inlineStr">
@@ -11373,12 +11373,12 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>E58.1B.DY2012</t>
+          <t>E58.1B.DY20-12</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>E58.1B.DY2012_Machida18S_osu867</t>
+          <t>E58.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D164" s="11" t="inlineStr">
@@ -11435,12 +11435,12 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>E58.2B.DY2012</t>
+          <t>E58.2B.DY20-12</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>E58.2B.DY2012_Machida18S_osu867</t>
+          <t>E58.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D165" s="11" t="inlineStr">
@@ -11497,12 +11497,12 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>E59.1B.DY2012</t>
+          <t>E59.1B.DY20-12</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>E59.1B.DY2012_Machida18S_osu867</t>
+          <t>E59.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D166" s="11" t="inlineStr">
@@ -11559,12 +11559,12 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>E59.2B.DY2012</t>
+          <t>E59.2B.DY20-12</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>E59.2B.DY2012_Machida18S_osu867</t>
+          <t>E59.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D167" s="11" t="inlineStr">
@@ -11621,12 +11621,12 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>E60.1B.DY2012</t>
+          <t>E60.1B.DY20-12</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>E60.1B.DY2012_Machida18S_osu867</t>
+          <t>E60.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D168" s="11" t="inlineStr">
@@ -11683,12 +11683,12 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>E60.2B.DY2012</t>
+          <t>E60.2B.DY20-12</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>E60.2B.DY2012_Machida18S_osu867</t>
+          <t>E60.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D169" s="11" t="inlineStr">
@@ -11745,12 +11745,12 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>E61.1B.DY2012</t>
+          <t>E61.1B.DY20-12</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>E61.1B.DY2012_Machida18S_osu867</t>
+          <t>E61.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D170" s="11" t="inlineStr">
@@ -11807,12 +11807,12 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>E61.2B.DY2012</t>
+          <t>E61.2B.DY20-12</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>E61.2B.DY2012_Machida18S_osu867</t>
+          <t>E61.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D171" s="11" t="inlineStr">
@@ -11869,12 +11869,12 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>E62.1B.DY2012</t>
+          <t>E62.1B.DY20-12</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>E62.1B.DY2012_Machida18S_osu867</t>
+          <t>E62.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D172" s="11" t="inlineStr">
@@ -11931,12 +11931,12 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>E62.2B.DY2012</t>
+          <t>E62.2B.DY20-12</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>E62.2B.DY2012_Machida18S_osu867</t>
+          <t>E62.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D173" s="11" t="inlineStr">
@@ -11993,12 +11993,12 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>E63.1B.DY2012</t>
+          <t>E63.1B.DY20-12</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>E63.1B.DY2012_Machida18S_osu867</t>
+          <t>E63.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D174" s="11" t="inlineStr">
@@ -12055,12 +12055,12 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>E63.2B.DY2012</t>
+          <t>E63.2B.DY20-12</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>E63.2B.DY2012_Machida18S_osu867</t>
+          <t>E63.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D175" s="11" t="inlineStr">
@@ -12117,12 +12117,12 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>E64.1B.DY2012</t>
+          <t>E64.1B.DY20-12</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>E64.1B.DY2012_Machida18S_osu867</t>
+          <t>E64.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D176" s="11" t="inlineStr">
@@ -12179,12 +12179,12 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>E64.2B.DY2012</t>
+          <t>E64.2B.DY20-12</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>E64.2B.DY2012_Machida18S_osu867</t>
+          <t>E64.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D177" s="11" t="inlineStr">
@@ -12241,12 +12241,12 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>E65.1B.DY2012</t>
+          <t>E65.1B.DY20-12</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>E65.1B.DY2012_Machida18S_osu867</t>
+          <t>E65.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D178" s="11" t="inlineStr">
@@ -12303,12 +12303,12 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>E65.2B.DY2012</t>
+          <t>E65.2B.DY20-12</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>E65.2B.DY2012_Machida18S_osu867</t>
+          <t>E65.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D179" s="11" t="inlineStr">
@@ -12365,12 +12365,12 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>E66.1B.DY2012</t>
+          <t>E66.1B.DY20-12</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>E66.1B.DY2012_Machida18S_osu867</t>
+          <t>E66.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D180" s="11" t="inlineStr">
@@ -12427,12 +12427,12 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>E66.2B.DY2012</t>
+          <t>E66.2B.DY20-12</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>E66.2B.DY2012_Machida18S_osu867</t>
+          <t>E66.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D181" s="11" t="inlineStr">
@@ -12489,12 +12489,12 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>E67.1B.DY2012</t>
+          <t>E67.1B.DY20-12</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>E67.1B.DY2012_Machida18S_osu867</t>
+          <t>E67.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D182" s="11" t="inlineStr">
@@ -12551,12 +12551,12 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>E67.2B.DY2012</t>
+          <t>E67.2B.DY20-12</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>E67.2B.DY2012_Machida18S_osu867</t>
+          <t>E67.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D183" s="11" t="inlineStr">
@@ -12613,12 +12613,12 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>E68.1B.DY2012</t>
+          <t>E68.1B.DY20-12</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>E68.1B.DY2012_Machida18S_osu867</t>
+          <t>E68.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D184" s="11" t="inlineStr">
@@ -12675,12 +12675,12 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>E68.2B.DY2012</t>
+          <t>E68.2B.DY20-12</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>E68.2B.DY2012_Machida18S_osu867</t>
+          <t>E68.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D185" s="11" t="inlineStr">
@@ -12737,12 +12737,12 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>E69.1B.DY2012</t>
+          <t>E69.1B.DY20-12</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>E69.1B.DY2012_Machida18S_osu867</t>
+          <t>E69.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D186" s="11" t="inlineStr">
@@ -12799,12 +12799,12 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>E69.2B.DY2012</t>
+          <t>E69.2B.DY20-12</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>E69.2B.DY2012_Machida18S_osu867</t>
+          <t>E69.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D187" s="11" t="inlineStr">
@@ -12861,12 +12861,12 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>E70.1B.DY2012</t>
+          <t>E70.1B.DY20-12</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>E70.1B.DY2012_Machida18S_osu867</t>
+          <t>E70.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D188" s="11" t="inlineStr">
@@ -12923,12 +12923,12 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>E70.2B.DY2012</t>
+          <t>E70.2B.DY20-12</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>E70.2B.DY2012_Machida18S_osu867</t>
+          <t>E70.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D189" s="11" t="inlineStr">
@@ -12985,12 +12985,12 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>E71.1B.DY2012</t>
+          <t>E71.1B.DY20-12</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>E71.1B.DY2012_Machida18S_osu867</t>
+          <t>E71.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D190" s="11" t="inlineStr">
@@ -13047,12 +13047,12 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>E71.2B.DY2012</t>
+          <t>E71.2B.DY20-12</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>E71.2B.DY2012_Machida18S_osu867</t>
+          <t>E71.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D191" s="11" t="inlineStr">
@@ -13109,12 +13109,12 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>E72.1B.DY2012</t>
+          <t>E72.1B.DY20-12</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>E72.1B.DY2012_Machida18S_osu867</t>
+          <t>E72.1B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D192" s="11" t="inlineStr">
@@ -13171,12 +13171,12 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>E72.2B.DY2012</t>
+          <t>E72.2B.DY20-12</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>E72.2B.DY2012_Machida18S_osu867</t>
+          <t>E72.2B.DY20-12_Machida18S_osu867</t>
         </is>
       </c>
       <c r="D193" s="11" t="inlineStr">

</xml_diff>

<commit_message>
update for add SRR, SAMP, and PRJNA to osu ncbi runs
</commit_message>
<xml_diff>
--- a/runs/osu867/ncbi_mapping/ncbi_submission_data/osu867_SRA_metadata.xlsx
+++ b/runs/osu867/ncbi_mapping/ncbi_submission_data/osu867_SRA_metadata.xlsx
@@ -1213,7 +1213,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q286"/>
+  <dimension ref="A1:R286"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
@@ -1325,6 +1325,11 @@
           <t>fasta_file</t>
         </is>
       </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>srr_accession</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="18" t="inlineStr">
@@ -1759,6 +1764,11 @@
           <t>MP_E25_2B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>SRR24914067</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1821,6 +1831,11 @@
           <t>MP_E26_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>SRR24914092</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1945,6 +1960,11 @@
           <t>MP_E27_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>SRR25997770</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2007,6 +2027,11 @@
           <t>MP_E27_2B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>SRR24914063</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2069,6 +2094,11 @@
           <t>MP_E28_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>SRR24914055</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2193,6 +2223,11 @@
           <t>MP_E29_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>SRR24914066</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2317,6 +2352,11 @@
           <t>MP_E30_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>SRR24914091</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2441,6 +2481,11 @@
           <t>MP_E31_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>SRR24914065</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2565,6 +2610,11 @@
           <t>MP_E32_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>SRR24914090</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2689,6 +2739,11 @@
           <t>MP_E33_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>SRR24914064</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2813,6 +2868,11 @@
           <t>MP_E34_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>SRR24914089</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2937,6 +2997,11 @@
           <t>MP_E35_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>SRR24914062</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3061,6 +3126,11 @@
           <t>MP_E36_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>SRR25997769</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3123,6 +3193,11 @@
           <t>MP_E36_2B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>SRR24914054</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3185,6 +3260,11 @@
           <t>MP_E37_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>SRR24914060</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3309,6 +3389,11 @@
           <t>MP_E38_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>SRR24914053</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3433,6 +3518,11 @@
           <t>MP_E39_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>SRR24914050</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3557,6 +3647,11 @@
           <t>MP_E40_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>SRR24914057</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -3681,6 +3776,11 @@
           <t>MP_E42_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>SRR24914021</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -3805,6 +3905,11 @@
           <t>MP_E43_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>SRR24914048</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -3929,6 +4034,11 @@
           <t>MP_E44_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>SRR24914023</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -3991,6 +4101,11 @@
           <t>MP_E45_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>SRR24914043</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -4115,6 +4230,11 @@
           <t>MP_E46_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>SRR24914056</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -4177,6 +4297,11 @@
           <t>MP_E46_2B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>SRR25997762</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -4239,6 +4364,11 @@
           <t>MP_E47_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>SRR24914046</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -4363,6 +4493,11 @@
           <t>MP_E48_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>SRR24914116</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -4487,6 +4622,11 @@
           <t>MP_E49_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R52" t="inlineStr">
+        <is>
+          <t>SRR25997761</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -4549,6 +4689,11 @@
           <t>MP_E49_2B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R53" t="inlineStr">
+        <is>
+          <t>SRR24914038</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -4611,6 +4756,11 @@
           <t>MP_E50_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R54" t="inlineStr">
+        <is>
+          <t>SRR24914114</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -4735,6 +4885,11 @@
           <t>MP_E51_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R56" t="inlineStr">
+        <is>
+          <t>SRR24914036</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -4859,6 +5014,11 @@
           <t>MP_E52_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R58" t="inlineStr">
+        <is>
+          <t>SRR24914111</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -4983,6 +5143,11 @@
           <t>MP_E53_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R60" t="inlineStr">
+        <is>
+          <t>SRR25997760</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -5045,6 +5210,11 @@
           <t>MP_E53_2B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R61" t="inlineStr">
+        <is>
+          <t>SRR24914032</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -5107,6 +5277,11 @@
           <t>MP_E54_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R62" t="inlineStr">
+        <is>
+          <t>SRR25997759</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -5169,6 +5344,11 @@
           <t>MP_E54_2B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R63" t="inlineStr">
+        <is>
+          <t>SRR24914108</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -5231,6 +5411,11 @@
           <t>MP_E55_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R64" t="inlineStr">
+        <is>
+          <t>SRR24914030</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -5355,6 +5540,11 @@
           <t>MP_E57_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R66" t="inlineStr">
+        <is>
+          <t>SRR24914103</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -5479,6 +5669,11 @@
           <t>MP_E58_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R68" t="inlineStr">
+        <is>
+          <t>SRR25997758</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -5541,6 +5736,11 @@
           <t>MP_E58_2B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R69" t="inlineStr">
+        <is>
+          <t>SRR24914025</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -5603,6 +5803,11 @@
           <t>MP_E59_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R70" t="inlineStr">
+        <is>
+          <t>SRR24914105</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -5727,6 +5932,11 @@
           <t>MP_E60_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R72" t="inlineStr">
+        <is>
+          <t>SRR24914027</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -5851,6 +6061,11 @@
           <t>MP_E61_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R74" t="inlineStr">
+        <is>
+          <t>SRR24914106</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -5975,6 +6190,11 @@
           <t>MP_E62_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R76" t="inlineStr">
+        <is>
+          <t>SRR24914028</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -6099,6 +6319,11 @@
           <t>MP_E63_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R78" t="inlineStr">
+        <is>
+          <t>SRR24914107</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -6223,6 +6448,11 @@
           <t>MP_E64_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R80" t="inlineStr">
+        <is>
+          <t>SRR24914029</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -6347,6 +6577,11 @@
           <t>MP_E65_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R82" t="inlineStr">
+        <is>
+          <t>SRR24914102</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -6471,6 +6706,11 @@
           <t>MP_E66_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R84" t="inlineStr">
+        <is>
+          <t>SRR24914024</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -6595,6 +6835,11 @@
           <t>MP_E67_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R86" t="inlineStr">
+        <is>
+          <t>SRR24914097</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -6719,6 +6964,11 @@
           <t>MP_E68_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R88" t="inlineStr">
+        <is>
+          <t>SRR24914015</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -6843,6 +7093,11 @@
           <t>MP_E69_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R90" t="inlineStr">
+        <is>
+          <t>SRR24914095</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -6967,6 +7222,11 @@
           <t>MP_E70_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R92" t="inlineStr">
+        <is>
+          <t>SRR24914013</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -7091,6 +7351,11 @@
           <t>MP_E71_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R94" t="inlineStr">
+        <is>
+          <t>SRR24914059</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -7215,6 +7480,11 @@
           <t>MP_E72_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R96" t="inlineStr">
+        <is>
+          <t>SRR24914052</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -7711,6 +7981,11 @@
           <t>MP_E25_2B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R104" t="inlineStr">
+        <is>
+          <t>SRR24914123</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -7773,6 +8048,11 @@
           <t>MP_E26_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R105" t="inlineStr">
+        <is>
+          <t>SRR24913982</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -7959,6 +8239,11 @@
           <t>MP_E27_2B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R108" t="inlineStr">
+        <is>
+          <t>SRR24913985</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -8021,6 +8306,11 @@
           <t>MP_E28_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R109" t="inlineStr">
+        <is>
+          <t>SRR24913978</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -8145,6 +8435,11 @@
           <t>MP_E29_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R111" t="inlineStr">
+        <is>
+          <t>SRR24914122</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -8269,6 +8564,11 @@
           <t>MP_E30_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R113" t="inlineStr">
+        <is>
+          <t>SRR24913981</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -8393,6 +8693,11 @@
           <t>MP_E31_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R115" t="inlineStr">
+        <is>
+          <t>SRR24914007</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -8517,6 +8822,11 @@
           <t>MP_E32_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R117" t="inlineStr">
+        <is>
+          <t>SRR24913980</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -8641,6 +8951,11 @@
           <t>MP_E33_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R119" t="inlineStr">
+        <is>
+          <t>SRR24913996</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -8765,6 +9080,11 @@
           <t>MP_E34_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R121" t="inlineStr">
+        <is>
+          <t>SRR24913979</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -8889,6 +9209,11 @@
           <t>MP_E35_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R123" t="inlineStr">
+        <is>
+          <t>SRR24913974</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -9075,6 +9400,11 @@
           <t>MP_E36_2B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R126" t="inlineStr">
+        <is>
+          <t>SRR24913977</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -9137,6 +9467,11 @@
           <t>MP_E37_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R127" t="inlineStr">
+        <is>
+          <t>SRR24914080</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -9261,6 +9596,11 @@
           <t>MP_E38_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R129" t="inlineStr">
+        <is>
+          <t>SRR24913976</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -9385,6 +9725,11 @@
           <t>MP_E39_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R131" t="inlineStr">
+        <is>
+          <t>SRR24913972</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -9509,6 +9854,11 @@
           <t>MP_E40_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R133" t="inlineStr">
+        <is>
+          <t>SRR24914061</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -9633,6 +9983,11 @@
           <t>MP_E42_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R135" t="inlineStr">
+        <is>
+          <t>SRR24914110</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -9757,6 +10112,11 @@
           <t>MP_E43_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R137" t="inlineStr">
+        <is>
+          <t>SRR24913970</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -9881,6 +10241,11 @@
           <t>MP_E44_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R139" t="inlineStr">
+        <is>
+          <t>SRR24914034</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -9943,6 +10308,11 @@
           <t>MP_E45_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R140" t="inlineStr">
+        <is>
+          <t>SRR24913966</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -10067,6 +10437,11 @@
           <t>MP_E46_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R142" t="inlineStr">
+        <is>
+          <t>SRR24914088</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -10191,6 +10566,11 @@
           <t>MP_E47_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R144" t="inlineStr">
+        <is>
+          <t>SRR24913968</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -10315,6 +10695,11 @@
           <t>MP_E48_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R146" t="inlineStr">
+        <is>
+          <t>SRR24914006</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -10501,6 +10886,11 @@
           <t>MP_E49_2B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R149" t="inlineStr">
+        <is>
+          <t>SRR24914083</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -10563,6 +10953,11 @@
           <t>MP_E50_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R150" t="inlineStr">
+        <is>
+          <t>SRR24914004</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -10687,6 +11082,11 @@
           <t>MP_E51_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R152" t="inlineStr">
+        <is>
+          <t>SRR24914085</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -10811,6 +11211,11 @@
           <t>MP_E52_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R154" t="inlineStr">
+        <is>
+          <t>SRR24914001</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -10997,6 +11402,11 @@
           <t>MP_E53_2B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R157" t="inlineStr">
+        <is>
+          <t>SRR24913956</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -11121,6 +11531,11 @@
           <t>MP_E54_2B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R159" t="inlineStr">
+        <is>
+          <t>SRR24913999</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -11183,6 +11598,11 @@
           <t>MP_E55_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R160" t="inlineStr">
+        <is>
+          <t>SRR24913958</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -11307,6 +11727,11 @@
           <t>MP_E57_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R162" t="inlineStr">
+        <is>
+          <t>SRR24913993</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -11493,6 +11918,11 @@
           <t>MP_E58_2B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R165" t="inlineStr">
+        <is>
+          <t>SRR24914070</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -11555,6 +11985,11 @@
           <t>MP_E59_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R166" t="inlineStr">
+        <is>
+          <t>SRR24913995</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -11679,6 +12114,11 @@
           <t>MP_E60_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R168" t="inlineStr">
+        <is>
+          <t>SRR24913962</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -11803,6 +12243,11 @@
           <t>MP_E61_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R170" t="inlineStr">
+        <is>
+          <t>SRR24913997</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -11927,6 +12372,11 @@
           <t>MP_E62_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R172" t="inlineStr">
+        <is>
+          <t>SRR24913961</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -12051,6 +12501,11 @@
           <t>MP_E63_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R174" t="inlineStr">
+        <is>
+          <t>SRR24913998</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -12175,6 +12630,11 @@
           <t>MP_E64_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R176" t="inlineStr">
+        <is>
+          <t>SRR24913960</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -12299,6 +12759,11 @@
           <t>MP_E65_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R178" t="inlineStr">
+        <is>
+          <t>SRR24913992</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -12423,6 +12888,11 @@
           <t>MP_E66_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R180" t="inlineStr">
+        <is>
+          <t>SRR24914071</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -12547,6 +13017,11 @@
           <t>MP_E67_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R182" t="inlineStr">
+        <is>
+          <t>SRR24913988</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -12671,6 +13146,11 @@
           <t>MP_E68_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R184" t="inlineStr">
+        <is>
+          <t>SRR24914075</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -12795,6 +13275,11 @@
           <t>MP_E69_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R186" t="inlineStr">
+        <is>
+          <t>SRR24913986</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -12919,6 +13404,11 @@
           <t>MP_E70_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R188" t="inlineStr">
+        <is>
+          <t>SRR24914079</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -13043,6 +13533,11 @@
           <t>MP_E71_1B_DY20_R2.fastq.gz</t>
         </is>
       </c>
+      <c r="R190" t="inlineStr">
+        <is>
+          <t>SRR24913959</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -13165,6 +13660,11 @@
       <c r="M192" t="inlineStr">
         <is>
           <t>MP_E72_1B_DY20_R2.fastq.gz</t>
+        </is>
+      </c>
+      <c r="R192" t="inlineStr">
+        <is>
+          <t>SRR24913975</t>
         </is>
       </c>
     </row>

</xml_diff>